<commit_message>
Fix failing test for invalid gender error message
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal5-Files/FAL5-invalidGender.xlsx
+++ b/cypress/fixtures/Fal5-Files/FAL5-invalidGender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EDDD1C-F359-4CBE-80EC-6AC76DD60186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED872EB-F17E-47ED-AC50-E324A3242140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5444,7 +5444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5583,6 +5583,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5595,9 +5598,7 @@
     <xf numFmtId="49" fontId="14" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5984,7 +5985,7 @@
   <dimension ref="A1:AA978"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5"/>
@@ -6007,10 +6008,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -6034,20 +6035,20 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
       <c r="M2" s="9"/>
       <c r="Z2" s="10"/>
     </row>
@@ -6262,7 +6263,7 @@
       <c r="G8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="54" t="s">
         <v>1647</v>
       </c>
       <c r="I8" s="25" t="s">
@@ -6376,7 +6377,7 @@
       <c r="G11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="59" t="s">
         <v>1645</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -23563,11 +23564,11 @@
       <c r="B1" s="50" t="s">
         <v>1137</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>1138</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="15.5">
@@ -23577,9 +23578,9 @@
       <c r="B2" s="50" t="s">
         <v>1140</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="15.5">
@@ -23589,11 +23590,11 @@
       <c r="B3" s="50" t="s">
         <v>1142</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="58" t="s">
         <v>1143</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Fix for FAL5 error validation changes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal5-Files/FAL5-invalidGender.xlsx
+++ b/cypress/fixtures/Fal5-Files/FAL5-invalidGender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED872EB-F17E-47ED-AC50-E324A3242140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FF312F-D38A-49D2-928D-B6948F35E6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="LOCODES " sheetId="3" r:id="rId3"/>
     <sheet name="ISO 3-letter country codes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateCount="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -5586,6 +5586,7 @@
     <xf numFmtId="49" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5598,7 +5599,6 @@
     <xf numFmtId="49" fontId="14" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5985,7 +5985,7 @@
   <dimension ref="A1:AA978"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5"/>
@@ -6008,10 +6008,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -6035,20 +6035,20 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
       <c r="M2" s="9"/>
       <c r="Z2" s="10"/>
     </row>
@@ -6377,7 +6377,7 @@
       <c r="G11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="55" t="s">
         <v>1645</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -23564,11 +23564,11 @@
       <c r="B1" s="50" t="s">
         <v>1137</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>1138</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="15.5">
@@ -23578,9 +23578,9 @@
       <c r="B2" s="50" t="s">
         <v>1140</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="15.5">
@@ -23590,11 +23590,11 @@
       <c r="B3" s="50" t="s">
         <v>1142</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>1143</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">

</xml_diff>